<commit_message>
test: add FRI tab to replacement_service_upload_test and example.xlsx
</commit_message>
<xml_diff>
--- a/test/support/fixtures/xlsx/disruption_v2_live/example.xlsx
+++ b/test/support/fixtures/xlsx/disruption_v2_live/example.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mharty/git/arrow/test/support/fixtures/xlsx/disruption_v2_live/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kfirestack/Documents/src/github.com/mbta/arrow/test/support/fixtures/xlsx/disruption_v2_live/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9045A5AA-5B64-C149-BDCE-B0482AB6C279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF05E237-5D71-3D40-A2EE-D6273ABDB28A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-61480" yWindow="-3840" windowWidth="30240" windowHeight="18880" xr2:uid="{2187EAB2-AE31-4D22-BACB-80EA9DE1E015}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="51200" windowHeight="22500" activeTab="1" xr2:uid="{2187EAB2-AE31-4D22-BACB-80EA9DE1E015}"/>
   </bookViews>
   <sheets>
     <sheet name="WKDY headways and runtimes" sheetId="4" r:id="rId1"/>
-    <sheet name="SAT headways and runtimes" sheetId="5" r:id="rId2"/>
-    <sheet name="SUN headways and runtimes" sheetId="6" r:id="rId3"/>
+    <sheet name="FRI headways and runtimes" sheetId="7" r:id="rId2"/>
+    <sheet name="SAT headways and runtimes" sheetId="5" r:id="rId3"/>
+    <sheet name="SUN headways and runtimes" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="33">
   <si>
     <t>Start time</t>
   </si>
@@ -145,7 +146,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -227,7 +228,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -571,6 +572,402 @@
   </sheetPr>
   <dimension ref="A1:E24"/>
   <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="2" max="2" width="19.5" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" customWidth="1"/>
+    <col min="4" max="4" width="55.5" customWidth="1"/>
+    <col min="5" max="5" width="49.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="6">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3">
+        <v>40</v>
+      </c>
+      <c r="E2" s="3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3">
+        <v>45</v>
+      </c>
+      <c r="E3" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="6">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3">
+        <v>60</v>
+      </c>
+      <c r="E4" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="6">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3">
+        <v>70</v>
+      </c>
+      <c r="E5" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="6">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3">
+        <v>60</v>
+      </c>
+      <c r="E6" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="6">
+        <v>2</v>
+      </c>
+      <c r="D7" s="3">
+        <v>55</v>
+      </c>
+      <c r="E7" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="6">
+        <v>3</v>
+      </c>
+      <c r="D8" s="3">
+        <v>55</v>
+      </c>
+      <c r="E8" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="6">
+        <v>3</v>
+      </c>
+      <c r="D9" s="3">
+        <v>55</v>
+      </c>
+      <c r="E9" s="3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="6">
+        <v>3</v>
+      </c>
+      <c r="D10" s="3">
+        <v>55</v>
+      </c>
+      <c r="E10" s="3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="6">
+        <v>3</v>
+      </c>
+      <c r="D11" s="3">
+        <v>60</v>
+      </c>
+      <c r="E11" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="6">
+        <v>2</v>
+      </c>
+      <c r="D12" s="3">
+        <v>60</v>
+      </c>
+      <c r="E12" s="3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="6">
+        <v>2</v>
+      </c>
+      <c r="D13" s="3">
+        <v>60</v>
+      </c>
+      <c r="E13" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="6">
+        <v>2</v>
+      </c>
+      <c r="D14" s="3">
+        <v>60</v>
+      </c>
+      <c r="E14" s="3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="6">
+        <v>2</v>
+      </c>
+      <c r="D15" s="3">
+        <v>60</v>
+      </c>
+      <c r="E15" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="6">
+        <v>2</v>
+      </c>
+      <c r="D16" s="3">
+        <v>50</v>
+      </c>
+      <c r="E16" s="3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="6">
+        <v>4</v>
+      </c>
+      <c r="D17" s="3">
+        <v>50</v>
+      </c>
+      <c r="E17" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="6">
+        <v>4</v>
+      </c>
+      <c r="D18" s="3">
+        <v>50</v>
+      </c>
+      <c r="E18" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="6">
+        <v>4</v>
+      </c>
+      <c r="D19" s="3">
+        <v>45</v>
+      </c>
+      <c r="E19" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="6">
+        <v>5</v>
+      </c>
+      <c r="D20" s="3">
+        <v>45</v>
+      </c>
+      <c r="E20" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="6">
+        <v>4</v>
+      </c>
+      <c r="D21" s="3">
+        <v>40</v>
+      </c>
+      <c r="E21" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE980E54-7048-5745-AAF7-A38466F02627}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:E24"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -960,7 +1357,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04B2659B-0058-4863-828E-4834330DE3F8}">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
@@ -1356,7 +1753,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A91E8ECB-645E-4C7C-B54D-40F43487F2D5}">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
@@ -1753,6 +2150,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="9ac8c65e-24cc-4907-9a10-66b1170b57fa" xsi:nil="true"/>
@@ -1761,15 +2167,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2002,20 +2399,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA46E352-1983-4CFE-ABFE-F18FB5E48C0B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C457723D-4526-420E-9AFF-DF32F9694D3B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="9ac8c65e-24cc-4907-9a10-66b1170b57fa"/>
     <ds:schemaRef ds:uri="0db2d361-8471-4f04-ae28-f5b2bb432068"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA46E352-1983-4CFE-ABFE-F18FB5E48C0B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
feat: Implement Friday Tab Import For Replacement Service  (#1297)
* test: require "friday" attribute in `replacement_service` api response

* test: add `FRI` tab to `replacement_service_upload_test` and `example.xlsx`

* test: ensure friday tab is on timetable view

* feat: implement friday tab for replacement service
</commit_message>
<xml_diff>
--- a/test/support/fixtures/xlsx/disruption_v2_live/example.xlsx
+++ b/test/support/fixtures/xlsx/disruption_v2_live/example.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mharty/git/arrow/test/support/fixtures/xlsx/disruption_v2_live/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kfirestack/Documents/src/github.com/mbta/arrow/test/support/fixtures/xlsx/disruption_v2_live/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9045A5AA-5B64-C149-BDCE-B0482AB6C279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF05E237-5D71-3D40-A2EE-D6273ABDB28A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-61480" yWindow="-3840" windowWidth="30240" windowHeight="18880" xr2:uid="{2187EAB2-AE31-4D22-BACB-80EA9DE1E015}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="51200" windowHeight="22500" activeTab="1" xr2:uid="{2187EAB2-AE31-4D22-BACB-80EA9DE1E015}"/>
   </bookViews>
   <sheets>
     <sheet name="WKDY headways and runtimes" sheetId="4" r:id="rId1"/>
-    <sheet name="SAT headways and runtimes" sheetId="5" r:id="rId2"/>
-    <sheet name="SUN headways and runtimes" sheetId="6" r:id="rId3"/>
+    <sheet name="FRI headways and runtimes" sheetId="7" r:id="rId2"/>
+    <sheet name="SAT headways and runtimes" sheetId="5" r:id="rId3"/>
+    <sheet name="SUN headways and runtimes" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="33">
   <si>
     <t>Start time</t>
   </si>
@@ -145,7 +146,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -227,7 +228,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -571,6 +572,402 @@
   </sheetPr>
   <dimension ref="A1:E24"/>
   <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="2" max="2" width="19.5" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" customWidth="1"/>
+    <col min="4" max="4" width="55.5" customWidth="1"/>
+    <col min="5" max="5" width="49.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="6">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3">
+        <v>40</v>
+      </c>
+      <c r="E2" s="3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3">
+        <v>45</v>
+      </c>
+      <c r="E3" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="6">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3">
+        <v>60</v>
+      </c>
+      <c r="E4" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="6">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3">
+        <v>70</v>
+      </c>
+      <c r="E5" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="6">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3">
+        <v>60</v>
+      </c>
+      <c r="E6" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="6">
+        <v>2</v>
+      </c>
+      <c r="D7" s="3">
+        <v>55</v>
+      </c>
+      <c r="E7" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="6">
+        <v>3</v>
+      </c>
+      <c r="D8" s="3">
+        <v>55</v>
+      </c>
+      <c r="E8" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="6">
+        <v>3</v>
+      </c>
+      <c r="D9" s="3">
+        <v>55</v>
+      </c>
+      <c r="E9" s="3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="6">
+        <v>3</v>
+      </c>
+      <c r="D10" s="3">
+        <v>55</v>
+      </c>
+      <c r="E10" s="3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="6">
+        <v>3</v>
+      </c>
+      <c r="D11" s="3">
+        <v>60</v>
+      </c>
+      <c r="E11" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="6">
+        <v>2</v>
+      </c>
+      <c r="D12" s="3">
+        <v>60</v>
+      </c>
+      <c r="E12" s="3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="6">
+        <v>2</v>
+      </c>
+      <c r="D13" s="3">
+        <v>60</v>
+      </c>
+      <c r="E13" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="6">
+        <v>2</v>
+      </c>
+      <c r="D14" s="3">
+        <v>60</v>
+      </c>
+      <c r="E14" s="3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="6">
+        <v>2</v>
+      </c>
+      <c r="D15" s="3">
+        <v>60</v>
+      </c>
+      <c r="E15" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="6">
+        <v>2</v>
+      </c>
+      <c r="D16" s="3">
+        <v>50</v>
+      </c>
+      <c r="E16" s="3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="6">
+        <v>4</v>
+      </c>
+      <c r="D17" s="3">
+        <v>50</v>
+      </c>
+      <c r="E17" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="6">
+        <v>4</v>
+      </c>
+      <c r="D18" s="3">
+        <v>50</v>
+      </c>
+      <c r="E18" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="6">
+        <v>4</v>
+      </c>
+      <c r="D19" s="3">
+        <v>45</v>
+      </c>
+      <c r="E19" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="6">
+        <v>5</v>
+      </c>
+      <c r="D20" s="3">
+        <v>45</v>
+      </c>
+      <c r="E20" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="6">
+        <v>4</v>
+      </c>
+      <c r="D21" s="3">
+        <v>40</v>
+      </c>
+      <c r="E21" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE980E54-7048-5745-AAF7-A38466F02627}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:E24"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -960,7 +1357,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04B2659B-0058-4863-828E-4834330DE3F8}">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
@@ -1356,7 +1753,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A91E8ECB-645E-4C7C-B54D-40F43487F2D5}">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
@@ -1753,6 +2150,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="9ac8c65e-24cc-4907-9a10-66b1170b57fa" xsi:nil="true"/>
@@ -1761,15 +2167,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2002,20 +2399,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA46E352-1983-4CFE-ABFE-F18FB5E48C0B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C457723D-4526-420E-9AFF-DF32F9694D3B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="9ac8c65e-24cc-4907-9a10-66b1170b57fa"/>
     <ds:schemaRef ds:uri="0db2d361-8471-4f04-ae28-f5b2bb432068"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA46E352-1983-4CFE-ABFE-F18FB5E48C0B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>